<commit_message>
HW4 Figs and notebook
</commit_message>
<xml_diff>
--- a/Working/HW2_BoxModel_manual/starter_code/HW_02_visualization_example_hsieh.xlsx
+++ b/Working/HW2_BoxModel_manual/starter_code/HW_02_visualization_example_hsieh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnahh\Desktop\GW_Modeling\homework-hsiehdf\Working\HW2_BoxModel_manual\starter_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BD817D-602E-4ED4-B60E-DA2429024699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389832D7-2F15-411C-B3F6-9F7BF59DAFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E797DA87-9764-CF40-B10D-4CBD1F0C2290}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{E797DA87-9764-CF40-B10D-4CBD1F0C2290}"/>
   </bookViews>
   <sheets>
     <sheet name="bcf_1_edited" sheetId="3" r:id="rId1"/>
@@ -12270,7 +12270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E986F2-53D6-1C4D-B056-8DFA12526A7B}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -18941,10 +18941,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520DF9AE-552C-DA41-ACC0-54A27029221C}">
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -18952,12 +18952,12 @@
     <col min="3" max="4" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="5" customFormat="1" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:28" s="5" customFormat="1" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.6">
       <c r="C2">
         <v>1</v>
       </c>
@@ -19058,7 +19058,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.6">
       <c r="C3">
         <v>0</v>
       </c>
@@ -19159,7 +19159,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A4">
         <v>1</v>
       </c>
@@ -19241,8 +19241,12 @@
       <c r="AA4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB4">
+        <f>SUM(C4:AA4)</f>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A5">
         <v>2</v>
       </c>
@@ -19325,14 +19329,18 @@
       <c r="AA5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB5">
+        <f t="shared" ref="AB5:AB28" si="2">SUM(C5:AA5)</f>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A6">
         <f>A5+1</f>
         <v>3</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B28" si="2">B5+100</f>
+        <f t="shared" ref="B6:B28" si="3">B5+100</f>
         <v>200</v>
       </c>
       <c r="C6">
@@ -19410,14 +19418,18 @@
       <c r="AA6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB6">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A7">
-        <f t="shared" ref="A7:A28" si="3">A6+1</f>
+        <f t="shared" ref="A7:A28" si="4">A6+1</f>
         <v>4</v>
       </c>
       <c r="B7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
       <c r="C7">
@@ -19495,14 +19507,18 @@
       <c r="AA7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB7">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A8">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="B8">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="C8">
@@ -19580,14 +19596,18 @@
       <c r="AA8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB8">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A9">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="B9">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="2"/>
         <v>500</v>
       </c>
       <c r="C9">
@@ -19665,14 +19685,18 @@
       <c r="AA9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB9">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A10">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="B10">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="2"/>
         <v>600</v>
       </c>
       <c r="C10">
@@ -19750,14 +19774,18 @@
       <c r="AA10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB10">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A11">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="B11">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="2"/>
         <v>700</v>
       </c>
       <c r="C11">
@@ -19835,14 +19863,18 @@
       <c r="AA11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB11">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A12">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B12">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="2"/>
         <v>800</v>
       </c>
       <c r="C12">
@@ -19920,14 +19952,18 @@
       <c r="AA12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB12">
+        <f>SUM(C12:AA12)</f>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A13">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="B13">
         <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="2"/>
         <v>900</v>
       </c>
       <c r="C13">
@@ -20005,14 +20041,18 @@
       <c r="AA13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB13">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A14">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="B14">
         <f t="shared" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="C14">
@@ -20090,14 +20130,18 @@
       <c r="AA14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB14">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A15">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="B15">
         <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="2"/>
         <v>1100</v>
       </c>
       <c r="C15">
@@ -20175,14 +20219,18 @@
       <c r="AA15">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB15">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A16">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="B16">
         <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="2"/>
         <v>1200</v>
       </c>
       <c r="C16">
@@ -20260,14 +20308,18 @@
       <c r="AA16">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB16">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A17">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="B17">
         <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="2"/>
         <v>1300</v>
       </c>
       <c r="C17">
@@ -20345,14 +20397,18 @@
       <c r="AA17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB17">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A18">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="B18">
         <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="2"/>
         <v>1400</v>
       </c>
       <c r="C18">
@@ -20430,14 +20486,18 @@
       <c r="AA18">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB18">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A19">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="B19">
         <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="2"/>
         <v>1500</v>
       </c>
       <c r="C19">
@@ -20515,14 +20575,18 @@
       <c r="AA19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB19">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A20">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="B20">
         <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="2"/>
         <v>1600</v>
       </c>
       <c r="C20">
@@ -20600,14 +20664,18 @@
       <c r="AA20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB20">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A21">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="B21">
         <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="2"/>
         <v>1700</v>
       </c>
       <c r="C21">
@@ -20685,14 +20753,18 @@
       <c r="AA21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB21">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A22">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="B22">
         <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="C22">
@@ -20770,14 +20842,18 @@
       <c r="AA22">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB22">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A23">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="B23">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="2"/>
         <v>1900</v>
       </c>
       <c r="C23">
@@ -20855,14 +20931,18 @@
       <c r="AA23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB23">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A24">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="B24">
         <f t="shared" si="3"/>
-        <v>21</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="C24">
@@ -20940,14 +21020,18 @@
       <c r="AA24">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB24">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A25">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="B25">
         <f t="shared" si="3"/>
-        <v>22</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="2"/>
         <v>2100</v>
       </c>
       <c r="C25">
@@ -21025,14 +21109,18 @@
       <c r="AA25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB25">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A26">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="B26">
         <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="2"/>
         <v>2200</v>
       </c>
       <c r="C26">
@@ -21110,14 +21198,18 @@
       <c r="AA26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB26">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A27">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="B27">
         <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="2"/>
         <v>2300</v>
       </c>
       <c r="C27">
@@ -21195,14 +21287,18 @@
       <c r="AA27">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB27">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.6">
       <c r="A28">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="B28">
         <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="2"/>
         <v>2400</v>
       </c>
       <c r="C28">
@@ -21280,102 +21376,106 @@
       <c r="AA28">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.6">
+      <c r="AB28">
+        <f t="shared" si="2"/>
+        <v>309.28000000000009</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.6">
       <c r="D31">
-        <f t="shared" ref="D31:AA31" si="4">C28-D28</f>
+        <f t="shared" ref="D31:AA31" si="5">C28-D28</f>
         <v>0.11999999999999922</v>
       </c>
       <c r="E31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12000000000000099</v>
       </c>
       <c r="F31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
       <c r="G31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12000000000000099</v>
       </c>
       <c r="H31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
       <c r="I31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11000000000000121</v>
       </c>
       <c r="J31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
       <c r="K31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
       <c r="L31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12000000000000099</v>
       </c>
       <c r="M31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.66000000000000014</v>
       </c>
       <c r="N31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1899999999999995</v>
       </c>
       <c r="O31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.65000000000000036</v>
       </c>
       <c r="P31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12000000000000099</v>
       </c>
       <c r="R31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
       <c r="S31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12000000000000099</v>
       </c>
       <c r="T31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
       <c r="U31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
       <c r="V31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11000000000000121</v>
       </c>
       <c r="W31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
       <c r="X31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12000000000000099</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12000000000000099</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11999999999999922</v>
       </c>
     </row>

</xml_diff>